<commit_message>
Upload Ok sauf pour le remplacement, Consultation OK, MAJ en cours...
</commit_message>
<xml_diff>
--- a/uploads/Tables Syderep_V2.xlsx
+++ b/uploads/Tables Syderep_V2.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="450" windowWidth="18915" windowHeight="7545"/>
+    <workbookView xWindow="120" yWindow="450" windowWidth="18915" windowHeight="7545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
-    <sheet name="Pivots" sheetId="4" r:id="rId2"/>
-    <sheet name="Reprise" sheetId="2" r:id="rId3"/>
-    <sheet name="Questions" sheetId="3" r:id="rId4"/>
-    <sheet name="Feuil1" sheetId="5" r:id="rId5"/>
+    <sheet name="Feuil2" sheetId="6" r:id="rId2"/>
+    <sheet name="Pivots" sheetId="4" r:id="rId3"/>
+    <sheet name="Reprise" sheetId="2" r:id="rId4"/>
+    <sheet name="Questions" sheetId="3" r:id="rId5"/>
+    <sheet name="Feuil1" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Feuil1!$A$1:$B$286</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Pivots!$A$1:$J$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Feuil1!$A$1:$B$286</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Pivots!$A$1:$J$39</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tables!$A$1:$I$230</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="906">
   <si>
     <t>ACTEUR</t>
   </si>
@@ -4082,10 +4083,10 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozenSplit"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection sqref="A1:I1048576"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -9935,6 +9936,1870 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H81"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>736</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>737</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>278</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A2" s="63" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" s="63" t="s">
+        <v>648</v>
+      </c>
+      <c r="C2" s="64" t="s">
+        <v>289</v>
+      </c>
+      <c r="D2" s="64" t="s">
+        <v>306</v>
+      </c>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" s="55"/>
+      <c r="H2" s="61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="102" x14ac:dyDescent="0.25">
+      <c r="A3" s="53" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>805</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>803</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" s="53"/>
+      <c r="H3" s="61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A4" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>806</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>738</v>
+      </c>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="G4" s="53"/>
+      <c r="H4" s="61">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>738</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>800</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>739</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>742</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G7" s="35"/>
+      <c r="H7" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>742</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G8" s="35"/>
+      <c r="H8" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>809</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>742</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>810</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>802</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>317</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G12" s="33"/>
+      <c r="H12" s="31">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G13" s="33"/>
+      <c r="H13" s="31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>802</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>802</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>745</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>749</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>335</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>746</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>342</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>306</v>
+      </c>
+      <c r="E20" s="41"/>
+      <c r="F20" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="31">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>651</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>749</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>652</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>804</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G22" s="36"/>
+      <c r="H22" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>782</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G23" s="8"/>
+      <c r="H23" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>653</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>654</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G24" s="8"/>
+      <c r="H24" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>802</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="G25" s="8"/>
+      <c r="H25" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>306</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>288</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="G26" s="8"/>
+      <c r="H26" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G27" s="8"/>
+      <c r="H27" s="31">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>751</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G28" s="8"/>
+      <c r="H28" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="E29" s="23"/>
+      <c r="F29" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G29" s="8"/>
+      <c r="H29" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>753</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G30" s="8"/>
+      <c r="H30" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="42" t="s">
+        <v>362</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>792</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G31" s="37" t="s">
+        <v>791</v>
+      </c>
+      <c r="H31" s="31"/>
+    </row>
+    <row r="32" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>554</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>738</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>751</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G32" s="8"/>
+      <c r="H32" s="31"/>
+    </row>
+    <row r="33" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>812</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G33" s="8"/>
+      <c r="H33" s="31"/>
+    </row>
+    <row r="34" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E34" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G34" s="8"/>
+      <c r="H34" s="31"/>
+    </row>
+    <row r="35" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>306</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>288</v>
+      </c>
+      <c r="F35" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>796</v>
+      </c>
+      <c r="H35" s="31"/>
+    </row>
+    <row r="36" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E36" s="23" t="s">
+        <v>745</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G36" s="8"/>
+      <c r="H36" s="31"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="E37" s="23" t="s">
+        <v>804</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G37" s="8"/>
+      <c r="H37" s="31"/>
+    </row>
+    <row r="38" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>657</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>749</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G38" s="8"/>
+      <c r="H38" s="31"/>
+    </row>
+    <row r="39" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>657</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="E39" s="23" t="s">
+        <v>749</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G39" s="8"/>
+      <c r="H39" s="31"/>
+    </row>
+    <row r="40" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>534</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>535</v>
+      </c>
+      <c r="D40" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E40" s="23" t="s">
+        <v>781</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G40" s="8"/>
+      <c r="H40" s="31"/>
+    </row>
+    <row r="41" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>531</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="D41" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E41" s="23" t="s">
+        <v>780</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G41" s="8"/>
+      <c r="H41" s="31"/>
+    </row>
+    <row r="42" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>533</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E42" s="23" t="s">
+        <v>778</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G42" s="8"/>
+      <c r="H42" s="31"/>
+    </row>
+    <row r="43" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D43" s="28" t="s">
+        <v>738</v>
+      </c>
+      <c r="E43" s="28" t="s">
+        <v>797</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G43" s="8"/>
+      <c r="H43" s="31"/>
+    </row>
+    <row r="44" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="B44" s="29" t="s">
+        <v>798</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="D44" s="23" t="s">
+        <v>654</v>
+      </c>
+      <c r="E44" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G44" s="8"/>
+      <c r="H44" s="31"/>
+    </row>
+    <row r="45" spans="1:8" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="D45" s="23" t="s">
+        <v>744</v>
+      </c>
+      <c r="E45" s="23" t="s">
+        <v>751</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G45" s="8"/>
+      <c r="H45" s="31"/>
+    </row>
+    <row r="46" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D46" s="28" t="s">
+        <v>306</v>
+      </c>
+      <c r="E46" s="28" t="s">
+        <v>288</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G46" s="8"/>
+      <c r="H46" s="31"/>
+    </row>
+    <row r="47" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>658</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="D47" s="23" t="s">
+        <v>654</v>
+      </c>
+      <c r="E47" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G47" s="8"/>
+      <c r="H47" s="31"/>
+    </row>
+    <row r="48" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>658</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="D48" s="23" t="s">
+        <v>654</v>
+      </c>
+      <c r="E48" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G48" s="8"/>
+      <c r="H48" s="31"/>
+    </row>
+    <row r="49" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="C49" s="32" t="s">
+        <v>483</v>
+      </c>
+      <c r="D49" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="E49" s="23" t="s">
+        <v>784</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G49" s="8"/>
+      <c r="H49" s="31"/>
+    </row>
+    <row r="50" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D50" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E50" s="23" t="s">
+        <v>802</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G50" s="8"/>
+      <c r="H50" s="31"/>
+    </row>
+    <row r="51" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D51" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E51" s="23" t="s">
+        <v>743</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G51" s="8"/>
+      <c r="H51" s="31"/>
+    </row>
+    <row r="52" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="D52" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E52" s="23" t="s">
+        <v>802</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G52" s="8"/>
+      <c r="H52" s="31"/>
+    </row>
+    <row r="53" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>541</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="D53" s="23" t="s">
+        <v>654</v>
+      </c>
+      <c r="E53" s="23" t="s">
+        <v>751</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G53" s="8"/>
+      <c r="H53" s="31"/>
+    </row>
+    <row r="54" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>539</v>
+      </c>
+      <c r="D54" s="23" t="s">
+        <v>654</v>
+      </c>
+      <c r="E54" s="23" t="s">
+        <v>751</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G54" s="8"/>
+      <c r="H54" s="31"/>
+    </row>
+    <row r="55" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>543</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="D55" s="23" t="s">
+        <v>654</v>
+      </c>
+      <c r="E55" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G55" s="8"/>
+      <c r="H55" s="31"/>
+    </row>
+    <row r="56" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>540</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D56" s="23" t="s">
+        <v>654</v>
+      </c>
+      <c r="E56" s="23"/>
+      <c r="F56" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G56" s="8"/>
+      <c r="H56" s="31"/>
+    </row>
+    <row r="57" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>786</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="D57" s="23" t="s">
+        <v>744</v>
+      </c>
+      <c r="E57" s="23" t="s">
+        <v>751</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G57" s="8"/>
+      <c r="H57" s="31"/>
+    </row>
+    <row r="58" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="D58" s="23" t="s">
+        <v>654</v>
+      </c>
+      <c r="E58" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G58" s="8"/>
+      <c r="H58" s="31"/>
+    </row>
+    <row r="59" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="B59" s="53" t="s">
+        <v>451</v>
+      </c>
+      <c r="C59" s="19" t="s">
+        <v>892</v>
+      </c>
+      <c r="D59" s="19" t="s">
+        <v>738</v>
+      </c>
+      <c r="E59" s="19" t="s">
+        <v>776</v>
+      </c>
+      <c r="F59" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="G59" s="56"/>
+      <c r="H59" s="56"/>
+    </row>
+    <row r="60" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="B60" s="53" t="s">
+        <v>456</v>
+      </c>
+      <c r="C60" s="19" t="s">
+        <v>891</v>
+      </c>
+      <c r="D60" s="19" t="s">
+        <v>738</v>
+      </c>
+      <c r="E60" s="19" t="s">
+        <v>777</v>
+      </c>
+      <c r="F60" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="G60" s="56"/>
+      <c r="H60" s="56"/>
+    </row>
+    <row r="61" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A61" s="53" t="s">
+        <v>266</v>
+      </c>
+      <c r="B61" s="53" t="s">
+        <v>555</v>
+      </c>
+      <c r="C61" s="19" t="s">
+        <v>893</v>
+      </c>
+      <c r="D61" s="19" t="s">
+        <v>738</v>
+      </c>
+      <c r="E61" s="19" t="s">
+        <v>801</v>
+      </c>
+      <c r="F61" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="G61" s="56"/>
+      <c r="H61" s="56"/>
+    </row>
+    <row r="62" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="B62" s="53" t="s">
+        <v>452</v>
+      </c>
+      <c r="C62" s="19" t="s">
+        <v>894</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>738</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>745</v>
+      </c>
+      <c r="F62" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="G62" s="56"/>
+      <c r="H62" s="56"/>
+    </row>
+    <row r="63" spans="1:8" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D63" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="E63" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G63" s="8"/>
+      <c r="H63" s="31"/>
+    </row>
+    <row r="64" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D64" s="23" t="s">
+        <v>744</v>
+      </c>
+      <c r="E64" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G64" s="8"/>
+      <c r="H64" s="31"/>
+    </row>
+    <row r="65" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="B65" s="53" t="s">
+        <v>455</v>
+      </c>
+      <c r="C65" s="19" t="s">
+        <v>895</v>
+      </c>
+      <c r="D65" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="E65" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="F65" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="G65" s="56"/>
+      <c r="H65" s="56"/>
+    </row>
+    <row r="66" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="B66" s="53" t="s">
+        <v>457</v>
+      </c>
+      <c r="C66" s="19" t="s">
+        <v>896</v>
+      </c>
+      <c r="D66" s="19" t="s">
+        <v>738</v>
+      </c>
+      <c r="E66" s="19" t="s">
+        <v>776</v>
+      </c>
+      <c r="F66" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="G66" s="56"/>
+      <c r="H66" s="56"/>
+    </row>
+    <row r="67" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A67" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="B67" s="53" t="s">
+        <v>458</v>
+      </c>
+      <c r="C67" s="19" t="s">
+        <v>897</v>
+      </c>
+      <c r="D67" s="19" t="s">
+        <v>738</v>
+      </c>
+      <c r="E67" s="19" t="s">
+        <v>778</v>
+      </c>
+      <c r="F67" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="G67" s="56"/>
+      <c r="H67" s="56"/>
+    </row>
+    <row r="68" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D68" s="23" t="s">
+        <v>744</v>
+      </c>
+      <c r="E68" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G68" s="8"/>
+      <c r="H68" s="31"/>
+    </row>
+    <row r="69" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>788</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="D69" s="23" t="s">
+        <v>744</v>
+      </c>
+      <c r="E69" s="23" t="s">
+        <v>751</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G69" s="8"/>
+      <c r="H69" s="31"/>
+    </row>
+    <row r="70" spans="1:8" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="D70" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="E70" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G70" s="8"/>
+      <c r="H70" s="31"/>
+    </row>
+    <row r="71" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="D71" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="E71" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G71" s="8"/>
+      <c r="H71" s="31"/>
+    </row>
+    <row r="72" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D72" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E72" s="23" t="s">
+        <v>742</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G72" s="8"/>
+      <c r="H72" s="31"/>
+    </row>
+    <row r="73" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A73" s="53" t="s">
+        <v>270</v>
+      </c>
+      <c r="B73" s="53" t="s">
+        <v>297</v>
+      </c>
+      <c r="C73" s="19" t="s">
+        <v>898</v>
+      </c>
+      <c r="D73" s="19" t="s">
+        <v>738</v>
+      </c>
+      <c r="E73" s="19" t="s">
+        <v>801</v>
+      </c>
+      <c r="F73" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="G73" s="56"/>
+      <c r="H73" s="56"/>
+    </row>
+    <row r="74" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="B74" s="53" t="s">
+        <v>500</v>
+      </c>
+      <c r="C74" s="19" t="s">
+        <v>899</v>
+      </c>
+      <c r="D74" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="E74" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="F74" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="G74" s="56"/>
+      <c r="H74" s="56"/>
+    </row>
+    <row r="75" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>779</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D75" s="23" t="s">
+        <v>738</v>
+      </c>
+      <c r="E75" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G75" s="8"/>
+      <c r="H75" s="31"/>
+    </row>
+    <row r="76" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A76" s="53" t="s">
+        <v>123</v>
+      </c>
+      <c r="B76" s="53" t="s">
+        <v>464</v>
+      </c>
+      <c r="C76" s="19" t="s">
+        <v>900</v>
+      </c>
+      <c r="D76" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="E76" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="F76" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="G76" s="56"/>
+      <c r="H76" s="56"/>
+    </row>
+    <row r="77" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A77" s="53" t="s">
+        <v>125</v>
+      </c>
+      <c r="B77" s="53" t="s">
+        <v>501</v>
+      </c>
+      <c r="C77" s="19" t="s">
+        <v>901</v>
+      </c>
+      <c r="D77" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="E77" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="F77" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="G77" s="56"/>
+      <c r="H77" s="56"/>
+    </row>
+    <row r="78" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A78" s="53" t="s">
+        <v>126</v>
+      </c>
+      <c r="B78" s="53" t="s">
+        <v>466</v>
+      </c>
+      <c r="C78" s="19" t="s">
+        <v>902</v>
+      </c>
+      <c r="D78" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="E78" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="F78" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="G78" s="56"/>
+      <c r="H78" s="56"/>
+    </row>
+    <row r="79" spans="1:8" ht="102" x14ac:dyDescent="0.25">
+      <c r="A79" s="53" t="s">
+        <v>271</v>
+      </c>
+      <c r="B79" s="53" t="s">
+        <v>502</v>
+      </c>
+      <c r="C79" s="19" t="s">
+        <v>903</v>
+      </c>
+      <c r="D79" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="E79" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="F79" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="G79" s="56"/>
+      <c r="H79" s="56"/>
+    </row>
+    <row r="80" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="53" t="s">
+        <v>272</v>
+      </c>
+      <c r="B80" s="53" t="s">
+        <v>503</v>
+      </c>
+      <c r="C80" s="19" t="s">
+        <v>904</v>
+      </c>
+      <c r="D80" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="E80" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="F80" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="G80" s="56"/>
+      <c r="H80" s="56"/>
+    </row>
+    <row r="81" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D81" s="28" t="s">
+        <v>306</v>
+      </c>
+      <c r="E81" s="28" t="s">
+        <v>288</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G81" s="8" t="s">
+        <v>795</v>
+      </c>
+      <c r="H81" s="31"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J39"/>
   <sheetViews>
@@ -11068,7 +12933,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A218"/>
   <sheetViews>
@@ -11309,7 +13174,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -11363,7 +13228,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:B286"/>

</xml_diff>